<commit_message>
automatically adding a column
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/Python Tutorial Supplementary Materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/dev/python/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514228E9-0F2F-A943-BC09-EA2CF64602DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C23CA2-77EE-C941-9FC3-D301E7ED34A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>transaction_id</t>
   </si>
@@ -35,20 +30,11 @@
   <si>
     <t xml:space="preserve">price </t>
   </si>
-  <si>
-    <t>$9.98</t>
-  </si>
-  <si>
-    <t>$8.53</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00;[Red]\-[$$-C09]#,##0.00"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -78,8 +64,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -396,15 +382,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1025" width="11.5"/>
+    <col min="1" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
+    <col min="4" max="1025" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
@@ -414,7 +402,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -437,7 +425,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>6.95</v>
+        <v>6.65</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -448,7 +436,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>7.95</v>
+        <v>7.94</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -458,8 +446,8 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
+      <c r="C5" s="1">
+        <v>3.45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -469,16 +457,44 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C6" s="1">
+        <v>4.67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>1006</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.8699999999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>1007</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>